<commit_message>
[issue#0007] Implement XBM state machine details and add comments.
</commit_message>
<xml_diff>
--- a/Resources/Part2/Part2_Resources.xlsx
+++ b/Resources/Part2/Part2_Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_dev\Repository\CSC_MS\Resources\Part2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D64069C-0E6E-49AE-8349-3F52840BCF04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7442F4A6-5902-4D03-991B-D8A315BA1FDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{69235439-E537-4EFE-8BCE-9350B1A114A4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Alm</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Stm32Cube</t>
+  </si>
+  <si>
+    <t>feature_periodic.h</t>
   </si>
 </sst>
 </file>
@@ -153,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -259,11 +262,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -300,6 +314,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -687,17 +707,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02DB742-7F16-46DE-AA85-96801C702F10}">
-  <dimension ref="B2:J23"/>
+  <dimension ref="B2:J24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="5.85546875" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
@@ -890,7 +910,7 @@
     </row>
     <row r="21" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F21" s="5"/>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H21" s="7" t="s">
@@ -900,22 +920,31 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F22" s="9"/>
-      <c r="G22" s="10" t="s">
+      <c r="F22" s="5"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="7"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F23" s="9"/>
+      <c r="G23" s="10" t="s">
         <v>2</v>
-      </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="12"/>
-    </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F23" s="13"/>
-      <c r="G23" s="10" t="s">
-        <v>3</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F24" s="13"/>
+      <c r="G24" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[main] Update codetemplates.xml and Part2/Part2_Resources.xlsx
</commit_message>
<xml_diff>
--- a/Resources/Part2/Part2_Resources.xlsx
+++ b/Resources/Part2/Part2_Resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_dev\Repository\CSC_MS\Resources\Part2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F6BF07-3D10-4F88-B000-B12530FA92D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD2CCAA-C83E-4132-992D-8C58DAECE548}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="3" xr2:uid="{69235439-E537-4EFE-8BCE-9350B1A114A4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="2" xr2:uid="{69235439-E537-4EFE-8BCE-9350B1A114A4}"/>
   </bookViews>
   <sheets>
     <sheet name="FolderStructure" sheetId="1" r:id="rId1"/>
@@ -584,15 +584,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -625,6 +616,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
@@ -1418,17 +1418,17 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="23" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="37"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
@@ -1500,41 +1500,41 @@
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="24">
         <v>256</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7" s="24">
         <v>20</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="24" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="26">
         <f>SUM(D5:D7)*8</f>
         <v>6144</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
@@ -1548,7 +1548,7 @@
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
-      <c r="H9" s="26"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
@@ -1565,16 +1565,16 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="30" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1582,13 +1582,13 @@
       <c r="B13" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="29">
         <v>8.69</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="29">
         <v>13.77</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="29">
         <f>D13-C13</f>
         <v>5.08</v>
       </c>
@@ -1597,28 +1597,28 @@
       <c r="B14" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="29">
         <v>25.56</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="29">
         <v>29.85</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="29">
         <f>D14-C14</f>
         <v>4.2900000000000027</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="33" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1626,14 +1626,14 @@
       <c r="B17" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="29">
         <f>D13</f>
         <v>13.77</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="29">
         <v>13.78</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="29">
         <f>D17-C17</f>
         <v>9.9999999999997868E-3</v>
       </c>
@@ -1642,14 +1642,14 @@
       <c r="B18" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="29">
         <f>D14</f>
         <v>29.85</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="29">
         <v>30.36</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="29">
         <f>D18-C18</f>
         <v>0.50999999999999801</v>
       </c>
@@ -1667,8 +1667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81DB461-D787-4308-AC00-CB052DC78480}">
   <dimension ref="B2:C13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1689,34 +1689,34 @@
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="29">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="29">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="29">
         <f>($C$10*1000*1000/(($C$12*1000)*($C$11+1)))-1</f>
         <v>1599</v>
       </c>
@@ -1732,7 +1732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6E367-B285-4A83-A182-1C6FF2035CBC}">
   <dimension ref="B2:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>

</xml_diff>